<commit_message>
updated circuit and parts
</commit_message>
<xml_diff>
--- a/Circuit/Pièces.xlsx
+++ b/Circuit/Pièces.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Nom</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Acheté</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
   </si>
   <si>
     <t>Con 5x2</t>
-  </si>
-  <si>
-    <t>X1</t>
   </si>
   <si>
     <t>Horloge du codec audio</t>
@@ -281,6 +272,18 @@
   </si>
   <si>
     <t>Connecteurs</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/e-switch/PS1040ABLK/EG2031-ND/46259</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/akm-semiconductor-inc/AK4556VT/974-1021-1-ND/2333407</t>
+  </si>
+  <si>
+    <t>U1,U2</t>
+  </si>
+  <si>
+    <t>Y1</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,22 +693,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -713,13 +716,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2">
@@ -727,83 +730,94 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>5.48</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>D3*E3</f>
+        <v>5.48</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3">
-        <f t="shared" ref="F3:F25" si="0">D3*E3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E4" s="3"/>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>44</v>
+        <f>D4*E4</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>D5*E5</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>14</v>
+      </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D6*E6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="J6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="J7" t="s">
-        <v>80</v>
+        <f>D7*E7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -811,17 +825,17 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>D8*E8</f>
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -829,101 +843,117 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
+      <c r="D9">
+        <v>1.58</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>44</v>
+        <f>D9*E9</f>
+        <v>1.58</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="J9" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
       <c r="D10">
-        <v>1.58</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>1.58</v>
+        <f>D10*E10</f>
+        <v>4.9800000000000004</v>
       </c>
       <c r="G10" s="3"/>
       <c r="J10" s="5" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
+      <c r="D11">
+        <v>7.99</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D11*E11</f>
+        <v>7.99</v>
       </c>
       <c r="G11" s="3"/>
+      <c r="J11" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <v>7.99</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>7.99</v>
+        <f>D12*E12</f>
+        <v>0</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="J12" s="5" t="s">
+      <c r="J12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>50</v>
+      <c r="A13" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>1.04</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D13*E13</f>
+        <v>3.12</v>
       </c>
       <c r="G13" s="3"/>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
@@ -932,221 +962,197 @@
         <v>46</v>
       </c>
       <c r="D14">
-        <v>1.04</v>
+        <v>1.27</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>3.12</v>
-      </c>
-      <c r="G14" s="3"/>
+        <f>D14*E14</f>
+        <v>1.27</v>
+      </c>
       <c r="J14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15">
-        <v>1.27</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>1.27</v>
-      </c>
-      <c r="J15" t="s">
-        <v>72</v>
-      </c>
+        <f>D15*E15</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f>D16*E16</f>
         <v>0</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f>D17*E17</f>
         <v>0</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f>D18*E18</f>
         <v>0</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f>D19*E19</f>
         <v>0</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20">
+        <v>32.020000000000003</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>D20*E20</f>
+        <v>32.020000000000003</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" t="s">
         <v>40</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21">
-        <v>32.020000000000003</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>32.020000000000003</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>44</v>
-      </c>
+        <f>D21*E21</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="3"/>
       <c r="J21" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
         <v>53</v>
       </c>
-      <c r="C22" t="s">
-        <v>54</v>
+      <c r="D22">
+        <v>2.84</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D22*E22</f>
+        <v>5.68</v>
       </c>
       <c r="G22" s="3"/>
       <c r="J22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
         <v>56</v>
       </c>
-      <c r="D23">
-        <v>2.84</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>5.68</v>
+        <f>D23*E23</f>
+        <v>0</v>
       </c>
       <c r="G23" s="3"/>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="E24" s="3"/>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f>D24*E24</f>
         <v>0</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1154,25 +1160,22 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
+      <c r="J28" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f>SUM(F2:F24)</f>
+        <v>62.120000000000005</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
       <c r="E29" s="3"/>
-      <c r="J29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <f>SUM(F2:F25)</f>
-        <v>51.660000000000004</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
@@ -1221,10 +1224,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1"/>
-    <hyperlink ref="J12" r:id="rId2"/>
+    <hyperlink ref="J9" r:id="rId1"/>
+    <hyperlink ref="J11" r:id="rId2"/>
+    <hyperlink ref="J10" r:id="rId3"/>
+    <hyperlink ref="J3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
circuit & part update
</commit_message>
<xml_diff>
--- a/Circuit/Pièces.xlsx
+++ b/Circuit/Pièces.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Laurent\Documents\GitHub\VHDL_GUITAR_PEDAL\Circuit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e1538867\Desktop\VHDL_GUITAR_PEDAL\VHDL_GUITAR_PEDAL\Circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
   <si>
     <t>Nom</t>
   </si>
@@ -53,19 +53,10 @@
     <t>AK4556</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
     <t>Régulateur 5V</t>
-  </si>
-  <si>
-    <t>Régulateur -5V</t>
   </si>
   <si>
     <t>Régulateur 3.3V</t>
@@ -259,18 +250,12 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>Asigned footprnt</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/yageo/RC0201FR-0710KL/311-10.0KMCT-ND/1948976</t>
   </si>
   <si>
     <t>à changer -&gt; non dispo en smt</t>
   </si>
   <si>
-    <t>50ma(codec) + 15ma(osc) + x ma(level translator)</t>
-  </si>
-  <si>
     <t>Connecteurs</t>
   </si>
   <si>
@@ -284,6 +269,36 @@
   </si>
   <si>
     <t>Y1</t>
+  </si>
+  <si>
+    <t>Footprint Name</t>
+  </si>
+  <si>
+    <t>U7,U8</t>
+  </si>
+  <si>
+    <t>AP2204</t>
+  </si>
+  <si>
+    <t>U4,U5</t>
+  </si>
+  <si>
+    <t>514-473-1458</t>
+  </si>
+  <si>
+    <t>C9,C10</t>
+  </si>
+  <si>
+    <t>Low ERS caps ( &lt;20ohm)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/diodes-incorporated/AZ1117CH-3.3TRG1/AZ1117CH-3.3TRG1DICT-ND/4505206</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/on-semiconductor/MC33275ST-5.0T3G/MC33275ST-5.0T3GOSCT-ND/1967094</t>
+  </si>
+  <si>
+    <t>Fuse</t>
   </si>
 </sst>
 </file>
@@ -664,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,22 +708,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -719,18 +734,18 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2">
-        <f>D2*E2</f>
+        <f t="shared" ref="F2:F4" si="0">D2*E2</f>
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -741,194 +756,217 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>5.48</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f>D3*E3</f>
-        <v>5.48</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
       <c r="F4">
-        <f>D4*E4</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="F5">
         <f>D5*E5</f>
         <v>0</v>
       </c>
+      <c r="G5" s="3"/>
+      <c r="J5" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F6">
         <f>D6*E6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="J6" t="s">
-        <v>77</v>
+      <c r="G6" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
       <c r="F7">
         <f>D7*E7</f>
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>1.58</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
       <c r="F8">
         <f>D8*E8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>41</v>
+        <v>1.58</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="J8" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9">
-        <v>1.58</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f>D9*E9</f>
-        <v>1.58</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="G9" s="3"/>
       <c r="J9" s="5" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
       <c r="D10">
-        <v>2.4900000000000002</v>
+        <v>7.99</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>4.9800000000000004</v>
+        <v>7.99</v>
       </c>
       <c r="G10" s="3"/>
       <c r="J10" s="5" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11">
-        <v>7.99</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F11">
         <f>D11*E11</f>
-        <v>7.99</v>
+        <v>0</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="J11" s="5" t="s">
+      <c r="J11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>47</v>
+      <c r="A12" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>1.04</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
       </c>
       <c r="F12">
         <f>D12*E12</f>
-        <v>0</v>
+        <v>3.12</v>
       </c>
       <c r="G12" s="3"/>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
@@ -937,50 +975,38 @@
         <v>43</v>
       </c>
       <c r="D13">
-        <v>1.04</v>
+        <v>1.27</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <f>D13*E13</f>
-        <v>3.12</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>1.27</v>
+      </c>
       <c r="J13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14">
-        <v>1.27</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F14">
         <f>D14*E14</f>
-        <v>1.27</v>
-      </c>
-      <c r="J14" t="s">
-        <v>69</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F15">
         <f>D15*E15</f>
@@ -990,10 +1016,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F16">
         <f>D16*E16</f>
@@ -1003,10 +1029,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
       </c>
       <c r="F17">
         <f>D17*E17</f>
@@ -1016,10 +1042,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
       </c>
       <c r="F18">
         <f>D18*E18</f>
@@ -1029,126 +1055,134 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
-        <v>37</v>
+      <c r="D19">
+        <v>32.020000000000003</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
       </c>
       <c r="F19">
         <f>D19*E19</f>
         <v>0</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D20">
-        <v>32.020000000000003</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20">
         <f>D20*E20</f>
-        <v>32.020000000000003</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="J20" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="s">
-        <v>51</v>
+      <c r="D21">
+        <v>2.84</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
       </c>
       <c r="F21">
         <f>D21*E21</f>
-        <v>0</v>
+        <v>5.68</v>
       </c>
       <c r="G21" s="3"/>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
         <v>53</v>
       </c>
-      <c r="D22">
-        <v>2.84</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
       <c r="F22">
         <f>D22*E22</f>
-        <v>5.68</v>
+        <v>0</v>
       </c>
       <c r="G22" s="3"/>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="E23" s="3"/>
       <c r="F23">
         <f>D23*E23</f>
         <v>0</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="J23" t="s">
-        <v>75</v>
+      <c r="G23" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24">
-        <f>D24*E24</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>78</v>
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -1156,26 +1190,26 @@
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
       <c r="E27" s="3"/>
+      <c r="J27" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <f>SUM(F2:F23)</f>
+        <v>26.62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
       <c r="E28" s="3"/>
-      <c r="J28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <f>SUM(F2:F24)</f>
-        <v>62.120000000000005</v>
-      </c>
-      <c r="D29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
@@ -1183,53 +1217,60 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J9" r:id="rId1"/>
-    <hyperlink ref="J11" r:id="rId2"/>
-    <hyperlink ref="J10" r:id="rId3"/>
+    <hyperlink ref="J8" r:id="rId1"/>
+    <hyperlink ref="J10" r:id="rId2"/>
+    <hyperlink ref="J9" r:id="rId3"/>
     <hyperlink ref="J3" r:id="rId4"/>
+    <hyperlink ref="J20" r:id="rId5"/>
+    <hyperlink ref="J19" r:id="rId6"/>
+    <hyperlink ref="J5" r:id="rId7"/>
+    <hyperlink ref="J4" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LCD Header v2 done
</commit_message>
<xml_diff>
--- a/Circuit/Pièces.xlsx
+++ b/Circuit/Pièces.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Laurent\Documents\GitHub\VHDL_GUITAR_PEDAL\Circuit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e1538867\Desktop\VHDL_GUITAR_PEDAL\VHDL_GUITAR_PEDAL\Circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3686689A-E788-4884-B85F-288FB9B488D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11850" windowHeight="4860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11850" windowHeight="4860"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="231">
   <si>
     <t>Nom</t>
   </si>
@@ -723,7 +722,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1215,11 +1214,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1296,9 @@
         <f t="shared" ref="G2:G16" si="0">E2*F2</f>
         <v>0.88</v>
       </c>
-      <c r="H2" s="19"/>
+      <c r="H2" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I2" s="24"/>
       <c r="J2" s="19"/>
       <c r="K2" s="15" t="s">
@@ -1437,7 +1438,9 @@
         <f t="shared" si="0"/>
         <v>0.83000000000000007</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I6" s="6" t="s">
         <v>38</v>
       </c>
@@ -1587,7 +1590,9 @@
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I10" s="6" t="s">
         <v>220</v>
       </c>
@@ -1623,7 +1628,9 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="H11" s="24"/>
+      <c r="H11" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I11" s="6" t="s">
         <v>223</v>
       </c>
@@ -1657,7 +1664,9 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="H12" s="24"/>
+      <c r="H12" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I12" s="6" t="s">
         <v>38</v>
       </c>
@@ -1691,7 +1700,9 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="H13" s="24"/>
+      <c r="H13" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I13" s="6" t="s">
         <v>38</v>
       </c>
@@ -1725,7 +1736,9 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I14" s="6" t="s">
         <v>38</v>
       </c>
@@ -1759,7 +1772,9 @@
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
-      <c r="H15" s="24"/>
+      <c r="H15" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I15" s="6" t="s">
         <v>38</v>
       </c>
@@ -1791,7 +1806,9 @@
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2470,7 +2487,9 @@
         <f>E37*F37</f>
         <v>0</v>
       </c>
-      <c r="H37" s="19"/>
+      <c r="H37" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I37" s="6" t="s">
         <v>38</v>
       </c>
@@ -2637,7 +2656,9 @@
         <f>E42*F42</f>
         <v>0</v>
       </c>
-      <c r="H42" s="19"/>
+      <c r="H42" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="I42" s="6" t="s">
         <v>38</v>
       </c>
@@ -3655,58 +3676,58 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L31" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L36" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L55" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L34" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="L18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="L57" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="L22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="L3" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="L4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="L5" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="L7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="L8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="L9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="L20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L23" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L24" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L26" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="L27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="L28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="L29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L30" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="L33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="L38" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="L39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="L43" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L44" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="L47" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L48" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="L56" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="L58" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="L59" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="L60" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="L61" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="L72" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="L46" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="L49" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="L70" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="L67" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="L68" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="L73" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="L64" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="L62" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="L63" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="L2" r:id="rId46" xr:uid="{DB224966-2A9C-49BB-88BB-D4BF0BC14DEB}"/>
-    <hyperlink ref="L16" r:id="rId47" xr:uid="{5FE7887D-E1BD-4682-B8A3-91ADE8C34389}"/>
-    <hyperlink ref="L12" r:id="rId48" xr:uid="{C8178BB5-A313-451C-84D3-585F2C12D612}"/>
-    <hyperlink ref="L13" r:id="rId49" xr:uid="{D5AB83EB-E3BF-4C73-863F-031574C580B1}"/>
-    <hyperlink ref="L10" r:id="rId50" xr:uid="{9795E9B6-30EF-42B3-B3B3-93EA8E6E524F}"/>
-    <hyperlink ref="L11" r:id="rId51" xr:uid="{285BAFD6-3B2B-43BC-A6B2-E4114D6088BA}"/>
-    <hyperlink ref="L6" r:id="rId52" xr:uid="{618C50AC-6A53-493C-9122-B8BC21942F21}"/>
+    <hyperlink ref="L31" r:id="rId1"/>
+    <hyperlink ref="L41" r:id="rId2"/>
+    <hyperlink ref="L36" r:id="rId3"/>
+    <hyperlink ref="L55" r:id="rId4"/>
+    <hyperlink ref="L34" r:id="rId5"/>
+    <hyperlink ref="L18" r:id="rId6"/>
+    <hyperlink ref="L57" r:id="rId7"/>
+    <hyperlink ref="L22" r:id="rId8"/>
+    <hyperlink ref="L3" r:id="rId9"/>
+    <hyperlink ref="L4" r:id="rId10"/>
+    <hyperlink ref="L5" r:id="rId11"/>
+    <hyperlink ref="L7" r:id="rId12"/>
+    <hyperlink ref="L8" r:id="rId13"/>
+    <hyperlink ref="L9" r:id="rId14"/>
+    <hyperlink ref="L19" r:id="rId15"/>
+    <hyperlink ref="L20" r:id="rId16"/>
+    <hyperlink ref="L23" r:id="rId17"/>
+    <hyperlink ref="L24" r:id="rId18"/>
+    <hyperlink ref="L26" r:id="rId19"/>
+    <hyperlink ref="L27" r:id="rId20"/>
+    <hyperlink ref="L28" r:id="rId21"/>
+    <hyperlink ref="L29" r:id="rId22"/>
+    <hyperlink ref="L30" r:id="rId23"/>
+    <hyperlink ref="L33" r:id="rId24"/>
+    <hyperlink ref="L38" r:id="rId25"/>
+    <hyperlink ref="L39" r:id="rId26"/>
+    <hyperlink ref="L43" r:id="rId27"/>
+    <hyperlink ref="L44" r:id="rId28"/>
+    <hyperlink ref="L47" r:id="rId29"/>
+    <hyperlink ref="L48" r:id="rId30"/>
+    <hyperlink ref="L56" r:id="rId31"/>
+    <hyperlink ref="L58" r:id="rId32"/>
+    <hyperlink ref="L59" r:id="rId33"/>
+    <hyperlink ref="L60" r:id="rId34"/>
+    <hyperlink ref="L61" r:id="rId35"/>
+    <hyperlink ref="L72" r:id="rId36"/>
+    <hyperlink ref="L46" r:id="rId37"/>
+    <hyperlink ref="L49" r:id="rId38"/>
+    <hyperlink ref="L70" r:id="rId39"/>
+    <hyperlink ref="L67" r:id="rId40"/>
+    <hyperlink ref="L68" r:id="rId41"/>
+    <hyperlink ref="L73" r:id="rId42"/>
+    <hyperlink ref="L64" r:id="rId43"/>
+    <hyperlink ref="L62" r:id="rId44"/>
+    <hyperlink ref="L63" r:id="rId45"/>
+    <hyperlink ref="L2" r:id="rId46"/>
+    <hyperlink ref="L16" r:id="rId47"/>
+    <hyperlink ref="L12" r:id="rId48"/>
+    <hyperlink ref="L13" r:id="rId49"/>
+    <hyperlink ref="L10" r:id="rId50"/>
+    <hyperlink ref="L11" r:id="rId51"/>
+    <hyperlink ref="L6" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>

</xml_diff>